<commit_message>
loyal customer page fixed
</commit_message>
<xml_diff>
--- a/test case excel/Test case of the website  final.xlsx
+++ b/test case excel/Test case of the website  final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesandu\OneDrive - Asia Pacific Institute of Information Technology\Documents\apiit\wdos-assignment-website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesandu\OneDrive - Asia Pacific Institute of Information Technology\Documents\apiit\wdos-assignment-website\test case excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A92971FF-91E9-4476-B725-5A949B00BAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0584CE78-7B66-4D6A-A960-B7F7F268BBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{64696745-3732-4B41-BF38-90CBF7DC39F6}"/>
   </bookViews>
@@ -277,7 +277,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,9 +411,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -420,8 +423,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,14 +453,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1589,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3CDA61-C93C-45E4-805E-AF3BB756D554}">
   <dimension ref="A1:P291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M250" workbookViewId="0">
-      <selection activeCell="Q294" sqref="Q294"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="73" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1607,465 +1613,465 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+      <c r="A9" s="5">
         <v>12</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="7"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A138" s="7" t="s">
+      <c r="A138" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B138" s="7"/>
-      <c r="C138" s="7"/>
-      <c r="D138" s="7"/>
-      <c r="E138" s="7"/>
-      <c r="F138" s="7"/>
-      <c r="G138" s="7"/>
-      <c r="H138" s="7"/>
-      <c r="I138" s="7"/>
-      <c r="J138" s="7"/>
-      <c r="K138" s="7"/>
-      <c r="L138" s="7"/>
-      <c r="M138" s="7"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
+      <c r="F138" s="8"/>
+      <c r="G138" s="8"/>
+      <c r="H138" s="8"/>
+      <c r="I138" s="8"/>
+      <c r="J138" s="8"/>
+      <c r="K138" s="8"/>
+      <c r="L138" s="8"/>
+      <c r="M138" s="8"/>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A139" s="7"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
-      <c r="G139" s="7"/>
-      <c r="H139" s="7"/>
-      <c r="I139" s="7"/>
-      <c r="J139" s="7"/>
-      <c r="K139" s="7"/>
-      <c r="L139" s="7"/>
-      <c r="M139" s="7"/>
+      <c r="A139" s="8"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="8"/>
+      <c r="D139" s="8"/>
+      <c r="E139" s="8"/>
+      <c r="F139" s="8"/>
+      <c r="G139" s="8"/>
+      <c r="H139" s="8"/>
+      <c r="I139" s="8"/>
+      <c r="J139" s="8"/>
+      <c r="K139" s="8"/>
+      <c r="L139" s="8"/>
+      <c r="M139" s="8"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A171" s="7" t="s">
+      <c r="A171" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B171" s="7"/>
-      <c r="C171" s="7"/>
-      <c r="D171" s="7"/>
-      <c r="E171" s="7"/>
-      <c r="F171" s="7"/>
-      <c r="G171" s="7"/>
-      <c r="H171" s="7"/>
-      <c r="I171" s="7"/>
+      <c r="B171" s="8"/>
+      <c r="C171" s="8"/>
+      <c r="D171" s="8"/>
+      <c r="E171" s="8"/>
+      <c r="F171" s="8"/>
+      <c r="G171" s="8"/>
+      <c r="H171" s="8"/>
+      <c r="I171" s="8"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A172" s="7"/>
-      <c r="B172" s="7"/>
-      <c r="C172" s="7"/>
-      <c r="D172" s="7"/>
-      <c r="E172" s="7"/>
-      <c r="F172" s="7"/>
-      <c r="G172" s="7"/>
-      <c r="H172" s="7"/>
-      <c r="I172" s="7"/>
+      <c r="A172" s="8"/>
+      <c r="B172" s="8"/>
+      <c r="C172" s="8"/>
+      <c r="D172" s="8"/>
+      <c r="E172" s="8"/>
+      <c r="F172" s="8"/>
+      <c r="G172" s="8"/>
+      <c r="H172" s="8"/>
+      <c r="I172" s="8"/>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" s="7" t="s">
+      <c r="A202" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B202" s="7"/>
-      <c r="C202" s="7"/>
-      <c r="D202" s="7"/>
-      <c r="E202" s="7"/>
-      <c r="F202" s="7"/>
-      <c r="G202" s="7"/>
-      <c r="H202" s="7"/>
-      <c r="I202" s="7"/>
+      <c r="B202" s="8"/>
+      <c r="C202" s="8"/>
+      <c r="D202" s="8"/>
+      <c r="E202" s="8"/>
+      <c r="F202" s="8"/>
+      <c r="G202" s="8"/>
+      <c r="H202" s="8"/>
+      <c r="I202" s="8"/>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A203" s="7"/>
-      <c r="B203" s="7"/>
-      <c r="C203" s="7"/>
-      <c r="D203" s="7"/>
-      <c r="E203" s="7"/>
-      <c r="F203" s="7"/>
-      <c r="G203" s="7"/>
-      <c r="H203" s="7"/>
-      <c r="I203" s="7"/>
+      <c r="A203" s="8"/>
+      <c r="B203" s="8"/>
+      <c r="C203" s="8"/>
+      <c r="D203" s="8"/>
+      <c r="E203" s="8"/>
+      <c r="F203" s="8"/>
+      <c r="G203" s="8"/>
+      <c r="H203" s="8"/>
+      <c r="I203" s="8"/>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A231" s="8" t="s">
+      <c r="A231" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B231" s="9"/>
-      <c r="C231" s="9"/>
-      <c r="D231" s="9"/>
-      <c r="E231" s="9"/>
-      <c r="F231" s="9"/>
-      <c r="G231" s="9"/>
-      <c r="H231" s="9"/>
-      <c r="I231" s="9"/>
-      <c r="J231" s="10"/>
+      <c r="B231" s="10"/>
+      <c r="C231" s="10"/>
+      <c r="D231" s="10"/>
+      <c r="E231" s="10"/>
+      <c r="F231" s="10"/>
+      <c r="G231" s="10"/>
+      <c r="H231" s="10"/>
+      <c r="I231" s="10"/>
+      <c r="J231" s="11"/>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A232" s="11"/>
-      <c r="B232" s="12"/>
-      <c r="C232" s="12"/>
-      <c r="D232" s="12"/>
-      <c r="E232" s="12"/>
-      <c r="F232" s="12"/>
-      <c r="G232" s="12"/>
-      <c r="H232" s="12"/>
-      <c r="I232" s="12"/>
-      <c r="J232" s="13"/>
+      <c r="A232" s="12"/>
+      <c r="B232" s="13"/>
+      <c r="C232" s="13"/>
+      <c r="D232" s="13"/>
+      <c r="E232" s="13"/>
+      <c r="F232" s="13"/>
+      <c r="G232" s="13"/>
+      <c r="H232" s="13"/>
+      <c r="I232" s="13"/>
+      <c r="J232" s="14"/>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A261" s="7" t="s">
+      <c r="A261" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B261" s="7"/>
-      <c r="C261" s="7"/>
-      <c r="D261" s="7"/>
-      <c r="E261" s="7"/>
-      <c r="F261" s="7"/>
-      <c r="G261" s="7"/>
-      <c r="H261" s="7"/>
-      <c r="I261" s="7"/>
+      <c r="B261" s="8"/>
+      <c r="C261" s="8"/>
+      <c r="D261" s="8"/>
+      <c r="E261" s="8"/>
+      <c r="F261" s="8"/>
+      <c r="G261" s="8"/>
+      <c r="H261" s="8"/>
+      <c r="I261" s="8"/>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A262" s="7"/>
-      <c r="B262" s="7"/>
-      <c r="C262" s="7"/>
-      <c r="D262" s="7"/>
-      <c r="E262" s="7"/>
-      <c r="F262" s="7"/>
-      <c r="G262" s="7"/>
-      <c r="H262" s="7"/>
-      <c r="I262" s="7"/>
+      <c r="A262" s="8"/>
+      <c r="B262" s="8"/>
+      <c r="C262" s="8"/>
+      <c r="D262" s="8"/>
+      <c r="E262" s="8"/>
+      <c r="F262" s="8"/>
+      <c r="G262" s="8"/>
+      <c r="H262" s="8"/>
+      <c r="I262" s="8"/>
     </row>
     <row r="291" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C291" t="s">

</xml_diff>